<commit_message>
Modified the pins for the hardware
- Simplified the pins for the device
- Remove grounds
</commit_message>
<xml_diff>
--- a/doc/raspi_pinout.xlsx
+++ b/doc/raspi_pinout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\word-clock\word-clock-raspberry\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\word-clock\word-clock-controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9FBADED8-69D1-4E4E-8A8F-88109CFDA00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{581C9406-E9E3-4566-B314-3DAB689D786F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D26893EB-391F-44EA-B883-E8C3530B30FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>SD Card Slot</t>
   </si>
@@ -165,9 +165,6 @@
     <t>LED (DATA)</t>
   </si>
   <si>
-    <t>LED (GND)</t>
-  </si>
-  <si>
     <t>RTC (VCC)</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
     <t>RADAR (DAT)</t>
   </si>
   <si>
-    <t>RADAR (GND)</t>
-  </si>
-  <si>
-    <t>RADAR (VCC)</t>
-  </si>
-  <si>
     <t>BRIGHTNESS (VCC)</t>
   </si>
   <si>
@@ -202,9 +193,6 @@
   </si>
   <si>
     <t>BRIGHTNESS (GND)</t>
-  </si>
-  <si>
-    <t>CENTRAL GROUND</t>
   </si>
   <si>
     <t>Seq</t>
@@ -324,9 +312,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -350,11 +335,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -471,27 +459,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -810,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A418BB92-6A4F-4F0E-9759-2FD5E3A2126A}">
-  <dimension ref="E3:O27"/>
+  <dimension ref="F3:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,589 +796,581 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="11"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>60</v>
+      <c r="I5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4</v>
+      </c>
+      <c r="L7" s="12">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="12">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4">
+        <v>5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>6</v>
+      </c>
+      <c r="L8" s="12">
+        <v>3</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="8" t="s">
+    </row>
+    <row r="9" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="9"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="12">
+        <v>4</v>
+      </c>
+      <c r="J9" s="4">
+        <v>7</v>
+      </c>
+      <c r="K9" s="4">
+        <v>8</v>
+      </c>
+      <c r="L9" s="12">
+        <v>4</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="12">
+        <v>5</v>
+      </c>
+      <c r="J10" s="4">
+        <v>9</v>
+      </c>
+      <c r="K10" s="4">
+        <v>10</v>
+      </c>
+      <c r="L10" s="12">
+        <v>5</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="12">
+        <v>6</v>
+      </c>
+      <c r="J11" s="4">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4">
+        <v>12</v>
+      </c>
+      <c r="L11" s="12">
+        <v>6</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="12">
+        <v>7</v>
+      </c>
+      <c r="J12" s="4">
+        <v>13</v>
+      </c>
+      <c r="K12" s="4">
+        <v>14</v>
+      </c>
+      <c r="L12" s="12">
+        <v>7</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="12">
+        <v>8</v>
+      </c>
+      <c r="J13" s="4">
+        <v>15</v>
+      </c>
+      <c r="K13" s="4">
+        <v>16</v>
+      </c>
+      <c r="L13" s="12">
+        <v>8</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="13">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="5">
+      <c r="I14" s="12">
+        <v>9</v>
+      </c>
+      <c r="J14" s="4">
+        <v>17</v>
+      </c>
+      <c r="K14" s="4">
+        <v>18</v>
+      </c>
+      <c r="L14" s="12">
+        <v>9</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+      <c r="G15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="12">
+        <v>10</v>
+      </c>
+      <c r="J15" s="4">
+        <v>19</v>
+      </c>
+      <c r="K15" s="4">
+        <v>20</v>
+      </c>
+      <c r="L15" s="12">
+        <v>10</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="13">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="9" t="s">
+      <c r="N15" s="3"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="12">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4">
+        <v>21</v>
+      </c>
+      <c r="K16" s="4">
+        <v>22</v>
+      </c>
+      <c r="L16" s="12">
+        <v>11</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+      <c r="G17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="12">
+        <v>12</v>
+      </c>
+      <c r="J17" s="4">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4">
+        <v>24</v>
+      </c>
+      <c r="L17" s="12">
+        <v>12</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="12">
+        <v>13</v>
+      </c>
+      <c r="J18" s="4">
+        <v>25</v>
+      </c>
+      <c r="K18" s="4">
+        <v>26</v>
+      </c>
+      <c r="L18" s="12">
+        <v>13</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F19" s="9"/>
+      <c r="G19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="12">
+        <v>14</v>
+      </c>
+      <c r="J19" s="4">
+        <v>27</v>
+      </c>
+      <c r="K19" s="4">
+        <v>28</v>
+      </c>
+      <c r="L19" s="12">
+        <v>14</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="12">
+        <v>15</v>
+      </c>
+      <c r="J20" s="4">
+        <v>29</v>
+      </c>
+      <c r="K20" s="4">
+        <v>30</v>
+      </c>
+      <c r="L20" s="12">
+        <v>15</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F21" s="9"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12">
+        <v>16</v>
+      </c>
+      <c r="J21" s="4">
+        <v>31</v>
+      </c>
+      <c r="K21" s="4">
         <v>32</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="L21" s="12">
+        <v>16</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="12">
+        <v>17</v>
+      </c>
+      <c r="J22" s="4">
+        <v>33</v>
+      </c>
+      <c r="K22" s="4">
+        <v>34</v>
+      </c>
+      <c r="L22" s="12">
+        <v>17</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="12">
+        <v>18</v>
+      </c>
+      <c r="J23" s="4">
+        <v>35</v>
+      </c>
+      <c r="K23" s="4">
+        <v>36</v>
+      </c>
+      <c r="L23" s="12">
+        <v>18</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="12">
+        <v>19</v>
+      </c>
+      <c r="J24" s="4">
+        <v>37</v>
+      </c>
+      <c r="K24" s="4">
+        <v>38</v>
+      </c>
+      <c r="L24" s="12">
+        <v>19</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="12">
+        <v>20</v>
+      </c>
+      <c r="J25" s="4">
         <v>39</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="13">
-        <v>2</v>
-      </c>
-      <c r="J7" s="5">
-        <v>3</v>
-      </c>
-      <c r="K7" s="5">
-        <v>4</v>
-      </c>
-      <c r="L7" s="13">
-        <v>2</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="10"/>
-    </row>
-    <row r="8" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="K25" s="4">
         <v>40</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="13">
-        <v>3</v>
-      </c>
-      <c r="J8" s="5">
-        <v>5</v>
-      </c>
-      <c r="K8" s="5">
-        <v>6</v>
-      </c>
-      <c r="L8" s="13">
-        <v>3</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="10" t="s">
+      <c r="L25" s="12">
+        <v>20</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J26" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F9" s="10"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="13">
-        <v>4</v>
-      </c>
-      <c r="J9" s="5">
-        <v>7</v>
-      </c>
-      <c r="K9" s="5">
-        <v>8</v>
-      </c>
-      <c r="L9" s="13">
-        <v>4</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="13">
-        <v>5</v>
-      </c>
-      <c r="J10" s="5">
-        <v>9</v>
-      </c>
-      <c r="K10" s="5">
-        <v>10</v>
-      </c>
-      <c r="L10" s="13">
-        <v>5</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="13">
-        <v>6</v>
-      </c>
-      <c r="J11" s="5">
-        <v>11</v>
-      </c>
-      <c r="K11" s="5">
-        <v>12</v>
-      </c>
-      <c r="L11" s="13">
-        <v>6</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O11" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="13">
-        <v>7</v>
-      </c>
-      <c r="J12" s="5">
-        <v>13</v>
-      </c>
-      <c r="K12" s="5">
-        <v>14</v>
-      </c>
-      <c r="L12" s="13">
-        <v>7</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F13" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="13">
-        <v>8</v>
-      </c>
-      <c r="J13" s="5">
-        <v>15</v>
-      </c>
-      <c r="K13" s="5">
-        <v>16</v>
-      </c>
-      <c r="L13" s="13">
-        <v>8</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="10"/>
-    </row>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="13">
-        <v>9</v>
-      </c>
-      <c r="J14" s="5">
-        <v>17</v>
-      </c>
-      <c r="K14" s="5">
-        <v>18</v>
-      </c>
-      <c r="L14" s="13">
-        <v>9</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="10"/>
-      <c r="G15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="13">
-        <v>10</v>
-      </c>
-      <c r="J15" s="5">
-        <v>19</v>
-      </c>
-      <c r="K15" s="5">
-        <v>20</v>
-      </c>
-      <c r="L15" s="13">
-        <v>10</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="10"/>
-      <c r="G16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="13">
-        <v>11</v>
-      </c>
-      <c r="J16" s="5">
-        <v>21</v>
-      </c>
-      <c r="K16" s="5">
-        <v>22</v>
-      </c>
-      <c r="L16" s="13">
-        <v>11</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="10"/>
-    </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F17" s="10"/>
-      <c r="G17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="13">
-        <v>12</v>
-      </c>
-      <c r="J17" s="5">
-        <v>23</v>
-      </c>
-      <c r="K17" s="5">
-        <v>24</v>
-      </c>
-      <c r="L17" s="13">
-        <v>12</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="10"/>
-    </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F18" s="10"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="13">
-        <v>13</v>
-      </c>
-      <c r="J18" s="5">
-        <v>25</v>
-      </c>
-      <c r="K18" s="5">
-        <v>26</v>
-      </c>
-      <c r="L18" s="13">
-        <v>13</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F19" s="10"/>
-      <c r="G19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="13">
-        <v>14</v>
-      </c>
-      <c r="J19" s="5">
-        <v>27</v>
-      </c>
-      <c r="K19" s="5">
-        <v>28</v>
-      </c>
-      <c r="L19" s="13">
-        <v>14</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O19" s="10"/>
-    </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F20" s="10"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="13">
-        <v>15</v>
-      </c>
-      <c r="J20" s="5">
-        <v>29</v>
-      </c>
-      <c r="K20" s="5">
-        <v>30</v>
-      </c>
-      <c r="L20" s="13">
-        <v>15</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F21" s="10"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="13">
-        <v>16</v>
-      </c>
-      <c r="J21" s="5">
-        <v>31</v>
-      </c>
-      <c r="K21" s="5">
-        <v>32</v>
-      </c>
-      <c r="L21" s="13">
-        <v>16</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="10"/>
-    </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F22" s="10"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="13">
-        <v>17</v>
-      </c>
-      <c r="J22" s="5">
-        <v>33</v>
-      </c>
-      <c r="K22" s="5">
-        <v>34</v>
-      </c>
-      <c r="L22" s="13">
-        <v>17</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="10"/>
-    </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F23" s="10"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="13">
-        <v>18</v>
-      </c>
-      <c r="J23" s="5">
-        <v>35</v>
-      </c>
-      <c r="K23" s="5">
-        <v>36</v>
-      </c>
-      <c r="L23" s="13">
-        <v>18</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F24" s="10"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="13">
-        <v>19</v>
-      </c>
-      <c r="J24" s="5">
-        <v>37</v>
-      </c>
-      <c r="K24" s="5">
-        <v>38</v>
-      </c>
-      <c r="L24" s="13">
-        <v>19</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F25" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" s="13">
-        <v>20</v>
-      </c>
-      <c r="J25" s="5">
-        <v>39</v>
-      </c>
-      <c r="K25" s="5">
-        <v>40</v>
-      </c>
-      <c r="L25" s="13">
-        <v>20</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N25" s="3"/>
-      <c r="O25" s="10"/>
-    </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="J26" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K26" s="4"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>